<commit_message>
FInished working on balance
</commit_message>
<xml_diff>
--- a/app/static/data/newCDMS.xlsx
+++ b/app/static/data/newCDMS.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="PROSPECT" sheetId="1" r:id="rId1"/>
-    <sheet name="STUDENTS" sheetId="2" r:id="rId2"/>
-    <sheet name="EX-STUDENT" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
@@ -66,6 +64,9 @@
     <t>Timothy Ojo</t>
   </si>
   <si>
+    <t>David Boris</t>
+  </si>
+  <si>
     <t>joeladewole3@gmail.com</t>
   </si>
   <si>
@@ -75,6 +76,9 @@
     <t>tojo@gmail.com</t>
   </si>
   <si>
+    <t>davebo@yahoo.com</t>
+  </si>
+  <si>
     <t>705957589</t>
   </si>
   <si>
@@ -102,6 +106,9 @@
     <t>FRSC</t>
   </si>
   <si>
+    <t>Finance</t>
+  </si>
+  <si>
     <t>Not-Interested</t>
   </si>
   <si>
@@ -115,108 +122,6 @@
   </si>
   <si>
     <t>This guy said he will pay asap</t>
-  </si>
-  <si>
-    <t>dob</t>
-  </si>
-  <si>
-    <t>courses</t>
-  </si>
-  <si>
-    <t>registration_fee</t>
-  </si>
-  <si>
-    <t>tutorial_fee</t>
-  </si>
-  <si>
-    <t>course_fee</t>
-  </si>
-  <si>
-    <t>payment_1</t>
-  </si>
-  <si>
-    <t>payment_2</t>
-  </si>
-  <si>
-    <t>payment_3</t>
-  </si>
-  <si>
-    <t>balance</t>
-  </si>
-  <si>
-    <t>exam</t>
-  </si>
-  <si>
-    <t>remark_1</t>
-  </si>
-  <si>
-    <t>remark_2</t>
-  </si>
-  <si>
-    <t>7059575819</t>
-  </si>
-  <si>
-    <t>Ikeja Lagos Nigeria</t>
-  </si>
-  <si>
-    <t>IPOI, IOK, KNIC</t>
-  </si>
-  <si>
-    <t>Fair</t>
-  </si>
-  <si>
-    <t>This guy is brilliant</t>
-  </si>
-  <si>
-    <t>He hasnt paid up all the money</t>
-  </si>
-  <si>
-    <t>results</t>
-  </si>
-  <si>
-    <t>referral_name</t>
-  </si>
-  <si>
-    <t>referral_number</t>
-  </si>
-  <si>
-    <t>referral_email</t>
-  </si>
-  <si>
-    <t>Sammy Posh</t>
-  </si>
-  <si>
-    <t>samy@posh.com</t>
-  </si>
-  <si>
-    <t>9740878636</t>
-  </si>
-  <si>
-    <t>IbSL, Posod</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
-    <t>Joe Boy</t>
-  </si>
-  <si>
-    <t>Timothy Foluso</t>
-  </si>
-  <si>
-    <t>9898857670</t>
-  </si>
-  <si>
-    <t>9048955737594</t>
-  </si>
-  <si>
-    <t>joe@boy.com</t>
-  </si>
-  <si>
-    <t>jorti@kb.com</t>
-  </si>
-  <si>
-    <t>The guy finish well</t>
   </si>
 </sst>
 </file>
@@ -574,7 +479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -629,22 +534,22 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -655,22 +560,22 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -681,283 +586,45 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
         <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2">
-        <v>8537493</v>
-      </c>
-      <c r="I2">
-        <v>343554</v>
-      </c>
-      <c r="J2">
-        <v>35457543</v>
-      </c>
-      <c r="K2">
-        <v>34342</v>
-      </c>
-      <c r="L2">
-        <v>34553</v>
-      </c>
-      <c r="M2">
-        <v>4686546</v>
-      </c>
-      <c r="N2">
-        <v>5558654</v>
-      </c>
-      <c r="O2" t="s">
-        <v>48</v>
-      </c>
-      <c r="P2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2">
-        <v>9900</v>
-      </c>
-      <c r="H2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J2" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3">
-        <v>49543</v>
-      </c>
-      <c r="H3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L3" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>